<commit_message>
test for card generators, update source tables
</commit_message>
<xml_diff>
--- a/Scripts/python/SourceTables/Eidolons.xlsx
+++ b/Scripts/python/SourceTables/Eidolons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\vscodespace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Obsidian\Perfect_World_Mobile_RU_Database\Scripts\python\SourceTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -647,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>